<commit_message>
Changes to use latest rates and format for PDF.
1) Display latest rates on rate index page.
2) Make sure we're using the most recent rate that is before the end of the billing period when generating reports.
3) Fix formatting on Student form so page breaks will be in the right places.
</commit_message>
<xml_diff>
--- a/SchoolDistrictBilling/wwwroot/reportTemplates/MonthlyIndividualStudent.xlsx
+++ b/SchoolDistrictBilling/wwwroot/reportTemplates/MonthlyIndividualStudent.xlsx
@@ -114,7 +114,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -170,6 +170,12 @@
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -859,10 +865,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -878,7 +887,7 @@
     <col min="11" max="11" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -893,7 +902,7 @@
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -908,7 +917,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -923,7 +932,7 @@
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -936,7 +945,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="12" t="s">
         <v>3</v>
@@ -951,7 +960,7 @@
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="12" t="s">
         <v>4</v>
@@ -968,7 +977,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -981,7 +990,7 @@
       <c r="J7" s="17"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="42"/>
       <c r="C8" s="43"/>
@@ -1002,7 +1011,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="48" t="s">
         <v>10</v>
@@ -1027,7 +1036,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="48" t="s">
         <v>16</v>
@@ -1058,7 +1067,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18"/>
       <c r="B11" s="52"/>
       <c r="C11" s="58"/>
@@ -1079,7 +1088,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="18"/>
       <c r="B12" s="19"/>
       <c r="C12" s="20"/>
@@ -1092,7 +1101,7 @@
       <c r="J12" s="26"/>
       <c r="K12" s="27"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18"/>
       <c r="B13" s="28">
         <v>1</v>
@@ -1107,7 +1116,7 @@
       <c r="J13" s="33"/>
       <c r="K13" s="35"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18"/>
       <c r="B14" s="28"/>
       <c r="C14" s="29"/>
@@ -1120,7 +1129,7 @@
       <c r="J14" s="33"/>
       <c r="K14" s="27"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18"/>
       <c r="B15" s="37"/>
       <c r="C15" s="38"/>
@@ -1133,7 +1142,7 @@
       <c r="J15" s="41"/>
       <c r="K15" s="35"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18"/>
       <c r="B16" s="19"/>
       <c r="C16" s="20"/>
@@ -1146,7 +1155,7 @@
       <c r="J16" s="26"/>
       <c r="K16" s="27"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18"/>
       <c r="B17" s="28">
         <f>B13+1</f>
@@ -1157,12 +1166,12 @@
       <c r="E17" s="31"/>
       <c r="F17" s="32"/>
       <c r="G17" s="33"/>
-      <c r="H17" s="36"/>
+      <c r="H17" s="34"/>
       <c r="I17" s="36"/>
       <c r="J17" s="33"/>
       <c r="K17" s="35"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18"/>
       <c r="B18" s="28"/>
       <c r="C18" s="29"/>
@@ -1175,7 +1184,7 @@
       <c r="J18" s="33"/>
       <c r="K18" s="27"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18"/>
       <c r="B19" s="37"/>
       <c r="C19" s="38"/>
@@ -1188,7 +1197,7 @@
       <c r="J19" s="41"/>
       <c r="K19" s="35"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18"/>
       <c r="B20" s="19"/>
       <c r="C20" s="20"/>
@@ -1201,7 +1210,7 @@
       <c r="J20" s="26"/>
       <c r="K20" s="27"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
       <c r="B21" s="28">
         <f>B17+1</f>
@@ -1212,12 +1221,12 @@
       <c r="E21" s="31"/>
       <c r="F21" s="32"/>
       <c r="G21" s="33"/>
-      <c r="H21" s="36"/>
+      <c r="H21" s="34"/>
       <c r="I21" s="36"/>
       <c r="J21" s="33"/>
       <c r="K21" s="35"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18"/>
       <c r="B22" s="28"/>
       <c r="C22" s="29"/>
@@ -1230,7 +1239,7 @@
       <c r="J22" s="33"/>
       <c r="K22" s="27"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
       <c r="B23" s="37"/>
       <c r="C23" s="38"/>
@@ -1243,7 +1252,7 @@
       <c r="J23" s="41"/>
       <c r="K23" s="35"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="18"/>
       <c r="B24" s="19"/>
       <c r="C24" s="20"/>
@@ -1256,7 +1265,7 @@
       <c r="J24" s="26"/>
       <c r="K24" s="25"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18"/>
       <c r="B25" s="28">
         <f>B21+1</f>
@@ -1267,12 +1276,12 @@
       <c r="E25" s="31"/>
       <c r="F25" s="32"/>
       <c r="G25" s="33"/>
-      <c r="H25" s="36"/>
+      <c r="H25" s="34"/>
       <c r="I25" s="36"/>
       <c r="J25" s="33"/>
       <c r="K25" s="35"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="18"/>
       <c r="B26" s="28"/>
       <c r="C26" s="29"/>
@@ -1285,7 +1294,7 @@
       <c r="J26" s="33"/>
       <c r="K26" s="25"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="18"/>
       <c r="B27" s="37"/>
       <c r="C27" s="38"/>
@@ -1298,7 +1307,7 @@
       <c r="J27" s="41"/>
       <c r="K27" s="35"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="18"/>
       <c r="B28" s="19"/>
       <c r="C28" s="20"/>
@@ -1311,7 +1320,7 @@
       <c r="J28" s="26"/>
       <c r="K28" s="25"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="18"/>
       <c r="B29" s="28">
         <f>B25+1</f>
@@ -1322,12 +1331,12 @@
       <c r="E29" s="31"/>
       <c r="F29" s="32"/>
       <c r="G29" s="33"/>
-      <c r="H29" s="36"/>
+      <c r="H29" s="34"/>
       <c r="I29" s="36"/>
       <c r="J29" s="33"/>
       <c r="K29" s="35"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="18"/>
       <c r="B30" s="28"/>
       <c r="C30" s="29"/>
@@ -1340,7 +1349,7 @@
       <c r="J30" s="33"/>
       <c r="K30" s="27"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="18"/>
       <c r="B31" s="37"/>
       <c r="C31" s="38"/>
@@ -1353,7 +1362,7 @@
       <c r="J31" s="41"/>
       <c r="K31" s="35"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="18"/>
       <c r="B32" s="19"/>
       <c r="C32" s="20"/>
@@ -1366,7 +1375,7 @@
       <c r="J32" s="26"/>
       <c r="K32" s="27"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="18"/>
       <c r="B33" s="28">
         <f>B29+1</f>
@@ -1377,12 +1386,12 @@
       <c r="E33" s="31"/>
       <c r="F33" s="32"/>
       <c r="G33" s="33"/>
-      <c r="H33" s="36"/>
+      <c r="H33" s="34"/>
       <c r="I33" s="36"/>
       <c r="J33" s="33"/>
       <c r="K33" s="35"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="18"/>
       <c r="B34" s="28"/>
       <c r="C34" s="29"/>
@@ -1395,7 +1404,7 @@
       <c r="J34" s="33"/>
       <c r="K34" s="27"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="18"/>
       <c r="B35" s="37"/>
       <c r="C35" s="38"/>
@@ -1408,7 +1417,7 @@
       <c r="J35" s="41"/>
       <c r="K35" s="35"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="18"/>
       <c r="B36" s="19"/>
       <c r="C36" s="20"/>
@@ -1421,7 +1430,7 @@
       <c r="J36" s="26"/>
       <c r="K36" s="27"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="18"/>
       <c r="B37" s="28">
         <f>B33+1</f>
@@ -1432,12 +1441,12 @@
       <c r="E37" s="31"/>
       <c r="F37" s="32"/>
       <c r="G37" s="33"/>
-      <c r="H37" s="36"/>
+      <c r="H37" s="34"/>
       <c r="I37" s="36"/>
       <c r="J37" s="33"/>
       <c r="K37" s="35"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="18"/>
       <c r="B38" s="28"/>
       <c r="C38" s="29"/>
@@ -1450,7 +1459,7 @@
       <c r="J38" s="33"/>
       <c r="K38" s="27"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="18"/>
       <c r="B39" s="37"/>
       <c r="C39" s="38"/>
@@ -1463,7 +1472,7 @@
       <c r="J39" s="41"/>
       <c r="K39" s="35"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="18"/>
       <c r="B40" s="19"/>
       <c r="C40" s="20"/>
@@ -1476,7 +1485,7 @@
       <c r="J40" s="26"/>
       <c r="K40" s="27"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="18"/>
       <c r="B41" s="28">
         <f>B37+1</f>
@@ -1487,12 +1496,12 @@
       <c r="E41" s="31"/>
       <c r="F41" s="32"/>
       <c r="G41" s="33"/>
-      <c r="H41" s="36"/>
+      <c r="H41" s="34"/>
       <c r="I41" s="36"/>
       <c r="J41" s="33"/>
       <c r="K41" s="35"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="18"/>
       <c r="B42" s="28"/>
       <c r="C42" s="29"/>
@@ -1505,7 +1514,7 @@
       <c r="J42" s="33"/>
       <c r="K42" s="27"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="18"/>
       <c r="B43" s="37"/>
       <c r="C43" s="38"/>
@@ -1519,7 +1528,8 @@
       <c r="K43" s="35"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to the report templates.
Updated the report templates for the 22-23 school year except for the year end reconciliation in case it's still being generated for last year. Add new files for the 21 versions just for backup.
</commit_message>
<xml_diff>
--- a/SchoolDistrictBilling/wwwroot/reportTemplates/MonthlyIndividualStudent.xlsx
+++ b/SchoolDistrictBilling/wwwroot/reportTemplates/MonthlyIndividualStudent.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\tools\omni\SchoolDistrictBilling\SchoolDistrictBilling\wwwroot\reportTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhensinger/dev/omnivest/SdBilling/SchoolDistrictBilling/wwwroot/reportTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0C8EA0-8803-416C-A0CE-FFDAE41771C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8775" yWindow="-27510" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8780" yWindow="-27520" windowWidth="21600" windowHeight="20240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,9 +31,6 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -42,9 +41,6 @@
     <t>( Charter School Name )</t>
   </si>
   <si>
-    <t>INVOICE FOR THE 2021-2022 SCHOOL YEAR</t>
-  </si>
-  <si>
     <t>Individual Student Information Sheet</t>
   </si>
   <si>
@@ -118,12 +114,15 @@
   </si>
   <si>
     <t>Prior</t>
+  </si>
+  <si>
+    <t>INVOICE FOR THE 2022-2023 SCHOOL YEAR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -924,31 +923,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.375" customWidth="1"/>
-    <col min="2" max="2" width="10.375" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
     <col min="4" max="4" width="25.5" customWidth="1"/>
     <col min="5" max="5" width="11" style="64" customWidth="1"/>
-    <col min="6" max="6" width="11.625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="9" style="64" customWidth="1"/>
-    <col min="9" max="9" width="10.125" style="64" customWidth="1"/>
-    <col min="10" max="10" width="9.125" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="64" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" customWidth="1"/>
     <col min="11" max="11" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -963,14 +962,14 @@
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
     </row>
-    <row r="2" spans="1:11" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="51"/>
       <c r="F2" s="6" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="51"/>
@@ -978,14 +977,14 @@
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="52"/>
       <c r="F3" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="52"/>
@@ -993,7 +992,7 @@
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
     </row>
-    <row r="4" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -1006,10 +1005,10 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
@@ -1021,10 +1020,10 @@
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
     </row>
-    <row r="6" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="12"/>
@@ -1035,10 +1034,10 @@
       <c r="I6" s="65"/>
       <c r="J6" s="12"/>
       <c r="K6" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="10" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1058,74 +1057,74 @@
       <c r="D8" s="38"/>
       <c r="E8" s="70"/>
       <c r="F8" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="39" t="s">
         <v>6</v>
-      </c>
-      <c r="G8" s="39" t="s">
-        <v>7</v>
       </c>
       <c r="H8" s="57"/>
       <c r="I8" s="66" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J8" s="39"/>
       <c r="K8" s="39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="41"/>
       <c r="D9" s="42"/>
       <c r="E9" s="71"/>
       <c r="F9" s="43"/>
       <c r="G9" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="58" t="s">
+      <c r="I9" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="58" t="s">
+      <c r="J9" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="44" t="s">
+      <c r="K9" s="45" t="s">
         <v>14</v>
-      </c>
-      <c r="K9" s="45" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="D10" s="41" t="s">
         <v>17</v>
-      </c>
-      <c r="D10" s="41" t="s">
-        <v>18</v>
       </c>
       <c r="E10" s="71"/>
       <c r="F10" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="40" t="s">
+      <c r="H10" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="58" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="67" t="s">
+      <c r="J10" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="J10" s="44" t="s">
-        <v>22</v>
-      </c>
       <c r="K10" s="39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -1136,20 +1135,20 @@
       <c r="E11" s="72"/>
       <c r="F11" s="43"/>
       <c r="G11" s="49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H11" s="59"/>
       <c r="I11" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="45" t="s">
+      <c r="K11" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="45" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="19"/>
       <c r="C12" s="20"/>
@@ -1162,7 +1161,7 @@
       <c r="J12" s="25"/>
       <c r="K12" s="26"/>
     </row>
-    <row r="13" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="27">
         <v>1</v>
@@ -1177,7 +1176,7 @@
       <c r="J13" s="31"/>
       <c r="K13" s="32"/>
     </row>
-    <row r="14" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="27"/>
       <c r="C14" s="28"/>
@@ -1190,7 +1189,7 @@
       <c r="J14" s="31"/>
       <c r="K14" s="26"/>
     </row>
-    <row r="15" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="33"/>
       <c r="C15" s="34"/>
@@ -1203,7 +1202,7 @@
       <c r="J15" s="36"/>
       <c r="K15" s="32"/>
     </row>
-    <row r="16" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="19"/>
       <c r="C16" s="20"/>
@@ -1216,7 +1215,7 @@
       <c r="J16" s="25"/>
       <c r="K16" s="26"/>
     </row>
-    <row r="17" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="27">
         <f>B13+1</f>
@@ -1232,7 +1231,7 @@
       <c r="J17" s="31"/>
       <c r="K17" s="32"/>
     </row>
-    <row r="18" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="B18" s="27"/>
       <c r="C18" s="28"/>
@@ -1245,7 +1244,7 @@
       <c r="J18" s="31"/>
       <c r="K18" s="26"/>
     </row>
-    <row r="19" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="33"/>
       <c r="C19" s="34"/>
@@ -1258,7 +1257,7 @@
       <c r="J19" s="36"/>
       <c r="K19" s="32"/>
     </row>
-    <row r="20" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
       <c r="B20" s="19"/>
       <c r="C20" s="20"/>
@@ -1271,7 +1270,7 @@
       <c r="J20" s="25"/>
       <c r="K20" s="26"/>
     </row>
-    <row r="21" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
       <c r="B21" s="27">
         <f>B17+1</f>
@@ -1287,7 +1286,7 @@
       <c r="J21" s="31"/>
       <c r="K21" s="32"/>
     </row>
-    <row r="22" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
       <c r="B22" s="27"/>
       <c r="C22" s="28"/>
@@ -1300,7 +1299,7 @@
       <c r="J22" s="31"/>
       <c r="K22" s="26"/>
     </row>
-    <row r="23" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="B23" s="33"/>
       <c r="C23" s="34"/>
@@ -1313,7 +1312,7 @@
       <c r="J23" s="36"/>
       <c r="K23" s="32"/>
     </row>
-    <row r="24" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="19"/>
       <c r="C24" s="20"/>
@@ -1326,7 +1325,7 @@
       <c r="J24" s="25"/>
       <c r="K24" s="24"/>
     </row>
-    <row r="25" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="27">
         <f>B21+1</f>
@@ -1342,7 +1341,7 @@
       <c r="J25" s="31"/>
       <c r="K25" s="32"/>
     </row>
-    <row r="26" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
       <c r="B26" s="27"/>
       <c r="C26" s="28"/>
@@ -1355,7 +1354,7 @@
       <c r="J26" s="31"/>
       <c r="K26" s="24"/>
     </row>
-    <row r="27" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="33"/>
       <c r="C27" s="34"/>
@@ -1368,7 +1367,7 @@
       <c r="J27" s="36"/>
       <c r="K27" s="32"/>
     </row>
-    <row r="28" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="19"/>
       <c r="C28" s="20"/>
@@ -1381,7 +1380,7 @@
       <c r="J28" s="25"/>
       <c r="K28" s="24"/>
     </row>
-    <row r="29" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="27">
         <f>B25+1</f>
@@ -1397,7 +1396,7 @@
       <c r="J29" s="31"/>
       <c r="K29" s="32"/>
     </row>
-    <row r="30" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
       <c r="B30" s="27"/>
       <c r="C30" s="28"/>
@@ -1410,7 +1409,7 @@
       <c r="J30" s="31"/>
       <c r="K30" s="26"/>
     </row>
-    <row r="31" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="33"/>
       <c r="C31" s="34"/>
@@ -1423,7 +1422,7 @@
       <c r="J31" s="36"/>
       <c r="K31" s="32"/>
     </row>
-    <row r="32" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
       <c r="B32" s="19"/>
       <c r="C32" s="20"/>
@@ -1436,7 +1435,7 @@
       <c r="J32" s="25"/>
       <c r="K32" s="26"/>
     </row>
-    <row r="33" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18"/>
       <c r="B33" s="27">
         <f>B29+1</f>
@@ -1452,7 +1451,7 @@
       <c r="J33" s="31"/>
       <c r="K33" s="32"/>
     </row>
-    <row r="34" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
       <c r="B34" s="27"/>
       <c r="C34" s="28"/>
@@ -1465,7 +1464,7 @@
       <c r="J34" s="31"/>
       <c r="K34" s="26"/>
     </row>
-    <row r="35" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
       <c r="B35" s="33"/>
       <c r="C35" s="34"/>
@@ -1478,7 +1477,7 @@
       <c r="J35" s="36"/>
       <c r="K35" s="32"/>
     </row>
-    <row r="36" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="18"/>
       <c r="B36" s="19"/>
       <c r="C36" s="20"/>
@@ -1491,7 +1490,7 @@
       <c r="J36" s="25"/>
       <c r="K36" s="26"/>
     </row>
-    <row r="37" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="18"/>
       <c r="B37" s="27">
         <f>B33+1</f>
@@ -1507,7 +1506,7 @@
       <c r="J37" s="31"/>
       <c r="K37" s="32"/>
     </row>
-    <row r="38" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="18"/>
       <c r="B38" s="27"/>
       <c r="C38" s="28"/>
@@ -1520,7 +1519,7 @@
       <c r="J38" s="31"/>
       <c r="K38" s="26"/>
     </row>
-    <row r="39" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="18"/>
       <c r="B39" s="33"/>
       <c r="C39" s="34"/>
@@ -1533,7 +1532,7 @@
       <c r="J39" s="36"/>
       <c r="K39" s="32"/>
     </row>
-    <row r="40" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="18"/>
       <c r="B40" s="19"/>
       <c r="C40" s="20"/>
@@ -1546,7 +1545,7 @@
       <c r="J40" s="25"/>
       <c r="K40" s="26"/>
     </row>
-    <row r="41" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="18"/>
       <c r="B41" s="27">
         <f>B37+1</f>
@@ -1562,7 +1561,7 @@
       <c r="J41" s="31"/>
       <c r="K41" s="32"/>
     </row>
-    <row r="42" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="18"/>
       <c r="B42" s="27"/>
       <c r="C42" s="28"/>
@@ -1575,7 +1574,7 @@
       <c r="J42" s="31"/>
       <c r="K42" s="26"/>
     </row>
-    <row r="43" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="18"/>
       <c r="B43" s="33"/>
       <c r="C43" s="34"/>

</xml_diff>

<commit_message>
Update all reports to the 2024-2025 year.
</commit_message>
<xml_diff>
--- a/SchoolDistrictBilling/wwwroot/reportTemplates/MonthlyIndividualStudent.xlsx
+++ b/SchoolDistrictBilling/wwwroot/reportTemplates/MonthlyIndividualStudent.xlsx
@@ -1,26 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhensinger/dev/omnivest/SdBilling/SchoolDistrictBilling/wwwroot/reportTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338E32B2-BFDF-DC47-9D8D-A2076733D67C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8780" yWindow="-27520" windowWidth="21600" windowHeight="20240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34200" windowHeight="22240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +27,12 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -116,13 +119,13 @@
     <t>Prior</t>
   </si>
   <si>
-    <t>INVOICE FOR THE 2022-2023 SCHOOL YEAR</t>
+    <t>INVOICE FOR THE 2024-2025 SCHOOL YEAR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -399,41 +402,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
@@ -443,19 +445,18 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -478,14 +479,14 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -500,67 +501,67 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -575,16 +576,16 @@
       <alignment shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -610,26 +611,26 @@
       <alignment horizontal="right" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -923,8 +924,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K43"/>
@@ -938,654 +939,640 @@
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
     <col min="4" max="4" width="25.5" customWidth="1"/>
-    <col min="5" max="5" width="11" style="64" customWidth="1"/>
+    <col min="5" max="5" width="11" style="62" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="9" style="64" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" style="64" customWidth="1"/>
+    <col min="8" max="8" width="9" style="62" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="62" customWidth="1"/>
     <col min="10" max="10" width="9.1640625" customWidth="1"/>
     <col min="11" max="11" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="4" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="6" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="9" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
     </row>
     <row r="6" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="15" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="10" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="1"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
     </row>
     <row r="8" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="37" t="s">
+      <c r="B8" s="35"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="57"/>
-      <c r="I8" s="66" t="s">
+      <c r="H8" s="55"/>
+      <c r="I8" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39" t="s">
+      <c r="J8" s="37"/>
+      <c r="K8" s="37" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="40" t="s">
+      <c r="C9" s="39"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="58" t="s">
+      <c r="H9" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="58" t="s">
+      <c r="I9" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="44" t="s">
+      <c r="J9" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="45" t="s">
+      <c r="K9" s="43" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="71"/>
-      <c r="F10" s="46" t="s">
+      <c r="E10" s="69"/>
+      <c r="F10" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="40" t="s">
+      <c r="G10" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="58" t="s">
+      <c r="H10" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="67" t="s">
+      <c r="I10" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="44" t="s">
+      <c r="J10" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="K10" s="39" t="s">
+      <c r="K10" s="37" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="43"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="49" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="59"/>
-      <c r="I11" s="68" t="s">
+      <c r="H11" s="57"/>
+      <c r="I11" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="45" t="s">
+      <c r="J11" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="45" t="s">
+      <c r="K11" s="43" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="26"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="24"/>
     </row>
     <row r="13" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="27">
+      <c r="A13" s="16"/>
+      <c r="B13" s="25">
         <v>1</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="32"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="30"/>
     </row>
     <row r="14" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="62"/>
-      <c r="I14" s="62"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="26"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="24"/>
     </row>
     <row r="15" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="32"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="30"/>
     </row>
     <row r="16" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="26"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="24"/>
     </row>
     <row r="17" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="27">
+      <c r="A17" s="16"/>
+      <c r="B17" s="25">
         <f>B13+1</f>
         <v>2</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="32"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="30"/>
     </row>
     <row r="18" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="62"/>
-      <c r="I18" s="62"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="26"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="24"/>
     </row>
     <row r="19" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="63"/>
-      <c r="I19" s="63"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="32"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="61"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="30"/>
     </row>
     <row r="20" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="60"/>
-      <c r="I20" s="60"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="26"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="24"/>
     </row>
     <row r="21" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="27">
+      <c r="A21" s="16"/>
+      <c r="B21" s="25">
         <f>B17+1</f>
         <v>3</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="61"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="32"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="60"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="30"/>
     </row>
     <row r="22" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="62"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="26"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="24"/>
     </row>
     <row r="23" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="75"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="63"/>
-      <c r="I23" s="63"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="32"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="30"/>
     </row>
     <row r="24" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="60"/>
-      <c r="I24" s="60"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="24"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="22"/>
     </row>
     <row r="25" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="27">
+      <c r="A25" s="16"/>
+      <c r="B25" s="25">
         <f>B21+1</f>
         <v>4</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="62"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="32"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="30"/>
     </row>
     <row r="26" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="74"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="24"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="22"/>
     </row>
     <row r="27" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="63"/>
-      <c r="I27" s="63"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="32"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="61"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="30"/>
     </row>
     <row r="28" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="60"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="24"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="58"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="22"/>
     </row>
     <row r="29" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="27">
+      <c r="A29" s="16"/>
+      <c r="B29" s="25">
         <f>B25+1</f>
         <v>5</v>
       </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="62"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="32"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="30"/>
     </row>
     <row r="30" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="62"/>
-      <c r="I30" s="62"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="26"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="72"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="24"/>
     </row>
     <row r="31" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="63"/>
-      <c r="I31" s="63"/>
-      <c r="J31" s="36"/>
-      <c r="K31" s="32"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="61"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="30"/>
     </row>
     <row r="32" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="73"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="60"/>
-      <c r="I32" s="60"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="26"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="58"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="24"/>
     </row>
     <row r="33" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="27">
+      <c r="A33" s="16"/>
+      <c r="B33" s="25">
         <f>B29+1</f>
         <v>6</v>
       </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="61"/>
-      <c r="I33" s="62"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="32"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="72"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="30"/>
     </row>
     <row r="34" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="74"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="62"/>
-      <c r="I34" s="62"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="26"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="72"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="60"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="24"/>
     </row>
     <row r="35" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="75"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="63"/>
-      <c r="I35" s="63"/>
-      <c r="J35" s="36"/>
-      <c r="K35" s="32"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="73"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="61"/>
+      <c r="I35" s="61"/>
+      <c r="J35" s="34"/>
+      <c r="K35" s="30"/>
     </row>
     <row r="36" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="18"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="73"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="60"/>
-      <c r="I36" s="60"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="26"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="71"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="58"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="24"/>
     </row>
     <row r="37" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="18"/>
-      <c r="B37" s="27">
+      <c r="A37" s="16"/>
+      <c r="B37" s="25">
         <f>B33+1</f>
         <v>7</v>
       </c>
-      <c r="C37" s="28"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="74"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="61"/>
-      <c r="I37" s="62"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="32"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="59"/>
+      <c r="I37" s="60"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="30"/>
     </row>
     <row r="38" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="18"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="74"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="62"/>
-      <c r="I38" s="62"/>
-      <c r="J38" s="31"/>
-      <c r="K38" s="26"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="72"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="60"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="24"/>
     </row>
     <row r="39" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="18"/>
-      <c r="B39" s="33"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="75"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="63"/>
-      <c r="I39" s="63"/>
-      <c r="J39" s="36"/>
-      <c r="K39" s="32"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="73"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
+      <c r="H39" s="61"/>
+      <c r="I39" s="61"/>
+      <c r="J39" s="34"/>
+      <c r="K39" s="30"/>
     </row>
     <row r="40" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="18"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="73"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="23"/>
-      <c r="H40" s="60"/>
-      <c r="I40" s="60"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="26"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="71"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="58"/>
+      <c r="I40" s="58"/>
+      <c r="J40" s="23"/>
+      <c r="K40" s="24"/>
     </row>
     <row r="41" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="18"/>
-      <c r="B41" s="27">
+      <c r="A41" s="16"/>
+      <c r="B41" s="25">
         <f>B37+1</f>
         <v>8</v>
       </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="74"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="61"/>
-      <c r="I41" s="62"/>
-      <c r="J41" s="31"/>
-      <c r="K41" s="32"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="72"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="59"/>
+      <c r="I41" s="60"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="30"/>
     </row>
     <row r="42" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="18"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="74"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="31"/>
-      <c r="H42" s="62"/>
-      <c r="I42" s="62"/>
-      <c r="J42" s="31"/>
-      <c r="K42" s="26"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="72"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="60"/>
+      <c r="I42" s="60"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="24"/>
     </row>
     <row r="43" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="18"/>
-      <c r="B43" s="33"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="75"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="63"/>
-      <c r="I43" s="63"/>
-      <c r="J43" s="36"/>
-      <c r="K43" s="32"/>
+      <c r="A43" s="16"/>
+      <c r="B43" s="31"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="73"/>
+      <c r="F43" s="34"/>
+      <c r="G43" s="34"/>
+      <c r="H43" s="61"/>
+      <c r="I43" s="61"/>
+      <c r="J43" s="34"/>
+      <c r="K43" s="30"/>
     </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>

</xml_diff>